<commit_message>
Finished up the README file
</commit_message>
<xml_diff>
--- a/dataset_stats.xlsx
+++ b/dataset_stats.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/PW_Gold_4TB/PXD017823_RTS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pwilmart/Box Sync/Github_misc/analysis_example_repos/PXD017823_Real-Time-Search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20847DCE-BFC4-564B-A186-CC3D609EA197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FCFE57-9EA6-8341-A300-4251CDE582A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60380" yWindow="1460" windowWidth="27360" windowHeight="19600" activeTab="4" xr2:uid="{E21F185A-E8F7-47D7-A5EE-95778AC152B6}"/>
   </bookViews>
@@ -314,7 +314,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="141">
   <si>
     <t>c06306_qy_RTS_3cell_2_A1.sqt</t>
   </si>
@@ -754,6 +754,9 @@
   </si>
   <si>
     <t>Totals</t>
+  </si>
+  <si>
+    <t>Gain over RTS</t>
   </si>
 </sst>
 </file>
@@ -9208,7 +9211,7 @@
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9985,10 +9988,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182E0173-AE73-BC49-BFBC-46DB2514765A}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9998,12 +10001,12 @@
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>107</v>
       </c>
@@ -10029,7 +10032,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>112</v>
       </c>
@@ -10057,7 +10060,7 @@
         <v>0.75686169500602496</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>117</v>
       </c>
@@ -10082,7 +10085,7 @@
         <v>0.77145534877493638</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>118</v>
       </c>
@@ -10107,7 +10110,7 @@
         <v>0.7944838666488151</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>114</v>
       </c>
@@ -10135,7 +10138,7 @@
         <v>0.75525505422412642</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>117</v>
       </c>
@@ -10160,7 +10163,7 @@
         <v>0.76877761413843881</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>118</v>
       </c>
@@ -10185,14 +10188,17 @@
         <v>0.79341277279421607</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="2"/>
+      <c r="J10" t="s">
+        <v>140</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>113</v>
       </c>
@@ -10219,8 +10225,12 @@
         <f t="shared" si="1"/>
         <v>0.79140447181684292</v>
       </c>
+      <c r="J11" s="2">
+        <f>(F11-F4)/F4</f>
+        <v>4.5639483460109674E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>117</v>
       </c>
@@ -10244,8 +10254,12 @@
         <f t="shared" si="1"/>
         <v>0.80117820324005895</v>
       </c>
+      <c r="J12" s="2">
+        <f t="shared" ref="J12:J13" si="2">(F12-F5)/F5</f>
+        <v>3.8528288788615063E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>118</v>
       </c>
@@ -10269,8 +10283,12 @@
         <f t="shared" si="1"/>
         <v>0.82059177935466598</v>
       </c>
+      <c r="J13" s="2">
+        <f t="shared" si="2"/>
+        <v>3.286147623862487E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>115</v>
       </c>
@@ -10298,7 +10316,7 @@
         <v>0.78993171776676929</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>117</v>
       </c>
@@ -10323,7 +10341,7 @@
         <v>0.80064265631275944</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>118</v>
       </c>

</xml_diff>